<commit_message>
modify system test file
</commit_message>
<xml_diff>
--- a/系统测试相关报告/MeetHere系统测试计划.xlsx
+++ b/系统测试相关报告/MeetHere系统测试计划.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84800D6B-ABA6-462E-91AB-86F2CAFD12C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462BAA6-A7F1-4640-A4DB-550908251AD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" tabRatio="521" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="220">
   <si>
     <t>预置条件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1161,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1232,16 +1232,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1637,12 +1628,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" ht="16.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -1739,7 +1730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9:H14"/>
     </sheetView>
   </sheetViews>
@@ -1756,52 +1747,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1810,92 +1801,92 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="33" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>118</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>117</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1904,80 +1895,80 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="33" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>182</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>117</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
@@ -3405,13 +3396,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -3554,8 +3545,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -3571,52 +3562,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -3625,50 +3616,50 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="38"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -3677,50 +3668,50 @@
       <c r="F6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="38"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="28"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -3729,50 +3720,50 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="38"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="28"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="38"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="33" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -3781,50 +3772,50 @@
       <c r="F12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A13" s="38"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="28"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="38"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="33" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -3833,50 +3824,50 @@
       <c r="F15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A16" s="38"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="28"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="38"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="33" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -3885,38 +3876,38 @@
       <c r="F18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A19" s="38"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="38"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
@@ -5279,17 +5270,23 @@
       <c r="H156" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A19"/>
+  <mergeCells count="44">
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C18:C20"/>
@@ -5298,12 +5295,12 @@
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
@@ -5330,8 +5327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -5347,52 +5344,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>82</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -5401,92 +5398,92 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>123</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -5495,92 +5492,92 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="33" t="s">
         <v>127</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -5589,92 +5586,92 @@
       <c r="F15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="36" t="s">
-        <v>132</v>
+      <c r="H15" s="33" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="33" t="s">
         <v>127</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -5683,120 +5680,120 @@
       <c r="F21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="33" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="3" t="s">
         <v>135</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="3" t="s">
         <v>113</v>
       </c>
       <c r="F28" s="3"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
     </row>
     <row r="29" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="33" t="s">
         <v>127</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -5805,92 +5802,92 @@
       <c r="F29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="33" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="3" t="s">
         <v>140</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F34" s="3"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
     </row>
     <row r="35" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="33" t="s">
         <v>127</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -5899,92 +5896,92 @@
       <c r="F35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G35" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="H35" s="36" t="s">
+      <c r="H35" s="33" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="3" t="s">
         <v>144</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
     </row>
     <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D41" s="33" t="s">
         <v>204</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -5993,92 +5990,92 @@
       <c r="F41" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="36" t="s">
+      <c r="G41" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="H41" s="36" t="s">
+      <c r="H41" s="33" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
       <c r="E42" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
     </row>
     <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
       <c r="E43" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
     </row>
     <row r="44" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
       <c r="E44" s="3" t="s">
         <v>205</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
     </row>
     <row r="45" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
       <c r="E45" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
       <c r="E46" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="33" t="s">
         <v>209</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -6087,80 +6084,80 @@
       <c r="F47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G47" s="36" t="s">
+      <c r="G47" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="H47" s="36" t="s">
+      <c r="H47" s="33" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
       <c r="E48" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
     </row>
     <row r="49" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
       <c r="E49" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
     </row>
     <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
       <c r="E50" s="3" t="s">
         <v>210</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
     </row>
     <row r="51" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
       <c r="E51" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
       <c r="E52" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F52" s="3"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="3"/>
@@ -7268,52 +7265,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -7322,92 +7319,92 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>150</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -7416,92 +7413,92 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="33" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -7510,92 +7507,92 @@
       <c r="F15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="33" t="s">
         <v>201</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -7604,80 +7601,80 @@
       <c r="F21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="3" t="s">
         <v>200</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
@@ -8974,7 +8971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:D34"/>
     </sheetView>
   </sheetViews>
@@ -8991,52 +8988,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>92</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -9045,92 +9042,92 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="33" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>158</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -9139,92 +9136,92 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="33" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>159</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="43" t="s">
         <v>158</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -9233,92 +9230,92 @@
       <c r="F15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="33" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="47"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="47"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="47"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="3" t="s">
         <v>163</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="47"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="47"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="43" t="s">
         <v>92</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -9327,92 +9324,92 @@
       <c r="F21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="33" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="47"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="44"/>
       <c r="E22" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="47"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="47"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="3" t="s">
         <v>186</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="47"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="44"/>
       <c r="E25" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="47"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="43" t="s">
         <v>92</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -9421,102 +9418,102 @@
       <c r="F27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="33" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="47"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="47"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="44"/>
       <c r="E29" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="47"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="44"/>
       <c r="E30" s="3" t="s">
         <v>159</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="36" x14ac:dyDescent="0.15">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="47"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.15">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="47"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="44"/>
       <c r="E32" s="3" t="s">
         <v>192</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="47"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="44"/>
       <c r="E33" s="3" t="s">
         <v>193</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="47"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="44"/>
       <c r="E34" s="3" t="s">
         <v>113</v>
       </c>
@@ -10776,7 +10773,7 @@
   <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -10792,50 +10789,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>96</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -10844,86 +10843,92 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>97</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="29" t="s">
+      <c r="B9" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>167</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -10932,76 +10937,80 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>168</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>98</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
@@ -12384,7 +12393,11 @@
       <c r="H152" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="G9:G14"/>
+    <mergeCell ref="H9:H14"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="D9:D14"/>
     <mergeCell ref="G1:G2"/>
@@ -12397,6 +12410,10 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="A3:A8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="B9:B14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12408,7 +12425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -12425,52 +12442,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>104</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -12479,92 +12496,92 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="33" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>105</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>104</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -12573,120 +12590,120 @@
       <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>105</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="3" t="s">
         <v>173</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="3" t="s">
         <v>112</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="3" t="s">
         <v>113</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="33" t="s">
         <v>216</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -12695,86 +12712,86 @@
       <c r="F17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A18" s="45"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="37"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A19" s="45"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="37"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A20" s="45"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="37"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="3" t="s">
         <v>217</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="45"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="37"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="45"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="30"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -12782,7 +12799,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
-      <c r="B24" s="49"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -14110,7 +14127,7 @@
   <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -14126,52 +14143,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>108</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -14180,120 +14197,120 @@
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="47" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="51"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="51"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3" t="s">
         <v>110</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="51"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="51"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="3" t="s">
         <v>111</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="51"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="3" t="s">
         <v>112</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="51"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="3" t="s">
         <v>113</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="52"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>178</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -14302,94 +14319,94 @@
       <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="33" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="3" t="s">
         <v>179</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="3" t="s">
         <v>112</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="48" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="45" t="s">
         <v>113</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="49"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="49"/>
+      <c r="D17" s="46"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="49"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="49"/>
+      <c r="D18" s="46"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>

</xml_diff>